<commit_message>
Added Excel To-Do List to main branch
</commit_message>
<xml_diff>
--- a/Excel-To-Do-List-.xlsx
+++ b/Excel-To-Do-List-.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Warushi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Warushi\Desktop\project_official\Tech-Care_official\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C0891B4-F36B-4299-B28B-24388DBFD654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08603F4C-12BC-4683-915E-DA232BEDF29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3660,7 +3660,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6"/>

</xml_diff>

<commit_message>
Updated Excel To-Do List with latest progress and status
</commit_message>
<xml_diff>
--- a/Excel-To-Do-List-.xlsx
+++ b/Excel-To-Do-List-.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Warushi\Desktop\project_official\Tech-Care_official\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08603F4C-12BC-4683-915E-DA232BEDF29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDCA87C-DAD4-4125-93AE-5C8F520BFFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -739,7 +739,7 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.10869565217391304</c:v>
+                  <c:v>0.14130434782608695</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1491,7 +1491,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1620,7 +1620,7 @@
               <a:cs typeface="Verdana"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>10.9%</a:t>
+            <a:t>14.1%</a:t>
           </a:fld>
           <a:endParaRPr lang="en-GB" sz="800" b="1" i="1">
             <a:solidFill>
@@ -3811,7 +3811,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="12.75" customHeight="1">
@@ -3859,7 +3859,7 @@
       </c>
       <c r="H10" s="1">
         <f>COUNTIFS($D$5:$D$29,$H$5,$E$5:$E$29,TRUE)*$I$5+COUNTIFS($D$5:$D$29,$H$6,$E$5:$E$29,TRUE)*$I$6+COUNTIFS($D$5:$D$29,$H$7,$E$5:$E$29,TRUE)*$I$7</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1">
@@ -3907,7 +3907,7 @@
       </c>
       <c r="H12" s="13">
         <f>IFERROR(H10/H11,0)</f>
-        <v>0.10869565217391304</v>
+        <v>0.14130434782608695</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1">

</xml_diff>